<commit_message>
add example of linear approximation
</commit_message>
<xml_diff>
--- a/sphinx-book/source/supervised/supervised/figures/linerexample.xlsx
+++ b/sphinx-book/source/supervised/supervised/figures/linerexample.xlsx
@@ -160,100 +160,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>8.6590788770635925</c:v>
+                  <c:v>8.0956983761338428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.2841430662631756</c:v>
+                  <c:v>6.3584709142937363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3933217202064716</c:v>
+                  <c:v>-9.0538699958343933</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8979213190034248</c:v>
+                  <c:v>-8.7182265748940431</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8921926260426432</c:v>
+                  <c:v>8.9200259897714638</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1365854752402385</c:v>
+                  <c:v>-9.3042265832076261</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.5407156045591925</c:v>
+                  <c:v>-4.4133448161558704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.7111883582101646</c:v>
+                  <c:v>9.2447384598757267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8529305486597103</c:v>
+                  <c:v>2.7177465556659968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4686404589964575</c:v>
+                  <c:v>5.8753709196157988</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2734870951730954</c:v>
+                  <c:v>-2.9620475485804487</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.4568148099960787</c:v>
+                  <c:v>-1.7930056336306706</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.7549126466105278</c:v>
+                  <c:v>-2.3413799644704358</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4216913545831105</c:v>
+                  <c:v>4.742625546582385</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.2352630892991865</c:v>
+                  <c:v>-2.0075984973084449</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.8692795334001531</c:v>
+                  <c:v>9.333353674828885</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3725470195343483</c:v>
+                  <c:v>2.570708236659776</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.48688608615028706</c:v>
+                  <c:v>-4.8462254027891838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.464469348912175</c:v>
+                  <c:v>2.5717899807409488</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.3344434387815713</c:v>
+                  <c:v>-9.0447708792058297</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.17238842880654204</c:v>
+                  <c:v>5.0938543900127939</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4220107422174273</c:v>
+                  <c:v>-5.6652526934797809</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.8313211790367916</c:v>
+                  <c:v>1.193065753965513</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.8655156333648719</c:v>
+                  <c:v>-8.7396015422229123</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7449628527101577</c:v>
+                  <c:v>-5.8504340646699493</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8983657636616886</c:v>
+                  <c:v>4.5563085794710005</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-5.0088238515256789</c:v>
+                  <c:v>-0.50986669413980401</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-6.6941104858112466</c:v>
+                  <c:v>-0.24261640966571107</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-8.8446258660020298</c:v>
+                  <c:v>7.9304074553934676</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-8.5624952762693809</c:v>
+                  <c:v>6.2014988414571981</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.1925021591615899</c:v>
+                  <c:v>-3.5243415840914105</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.45375608043095994</c:v>
+                  <c:v>6.0344773562181402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -265,100 +265,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>26.098233089866206</c:v>
+                  <c:v>23.516836372566999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.4406431562717383</c:v>
+                  <c:v>9.7927900537197523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.7197840831272853</c:v>
+                  <c:v>-39.964745723879041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0629258000806132</c:v>
+                  <c:v>-30.353108440276458</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1398363884129132</c:v>
+                  <c:v>26.166626012538096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36237316351905768</c:v>
+                  <c:v>-37.422312604455122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-26.830086708882241</c:v>
+                  <c:v>-18.035470189791202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-9.6931342909662224</c:v>
+                  <c:v>24.393674735037003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3015410595750883</c:v>
+                  <c:v>-4.5894989460333768</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7829670717939727</c:v>
+                  <c:v>15.703714798576476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.967522288170429</c:v>
+                  <c:v>-7.5080423854717271</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.631790614940769</c:v>
+                  <c:v>-11.815063330453654</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.404662155770986</c:v>
+                  <c:v>-14.963211243563213</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.947435153992171</c:v>
+                  <c:v>2.2820824770814472</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-19.503609558803056</c:v>
+                  <c:v>-5.0683059129149015</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.503590786188436</c:v>
+                  <c:v>28.449406423645499</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.466312913114884</c:v>
+                  <c:v>3.0863791540935406</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.1253638195594462</c:v>
+                  <c:v>-25.640957704063428</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-19.853455059597582</c:v>
+                  <c:v>7.7958445188613386</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.9977973057784144</c:v>
+                  <c:v>-26.250613886468429</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.16240902129444734</c:v>
+                  <c:v>8.1661960921313863</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.8716384069934957</c:v>
+                  <c:v>-21.992417135811777</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16.584886855573863</c:v>
+                  <c:v>0.69834744053311582</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.6389032708564546</c:v>
+                  <c:v>-31.963842249024765</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3589800872131814</c:v>
+                  <c:v>-17.519261579906498</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.7354206250785609</c:v>
+                  <c:v>9.8546287789354583</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-26.372431239146543</c:v>
+                  <c:v>-10.856846541179682</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-18.728556048011026</c:v>
+                  <c:v>-8.338762010397561</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-24.810507019038031</c:v>
+                  <c:v>19.568059472444205</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-38.556423042831128</c:v>
+                  <c:v>5.8368880554364218</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.56480865976764605</c:v>
+                  <c:v>-19.453280391876987</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-5.574559983498748</c:v>
+                  <c:v>19.152451294974313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,100 +390,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>8.6590788770635925</c:v>
+                  <c:v>8.0956983761338428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.2841430662631756</c:v>
+                  <c:v>6.3584709142937363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3933217202064716</c:v>
+                  <c:v>-9.0538699958343933</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8979213190034248</c:v>
+                  <c:v>-8.7182265748940431</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8921926260426432</c:v>
+                  <c:v>8.9200259897714638</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1365854752402385</c:v>
+                  <c:v>-9.3042265832076261</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.5407156045591925</c:v>
+                  <c:v>-4.4133448161558704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.7111883582101646</c:v>
+                  <c:v>9.2447384598757267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8529305486597103</c:v>
+                  <c:v>2.7177465556659968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4686404589964575</c:v>
+                  <c:v>5.8753709196157988</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2734870951730954</c:v>
+                  <c:v>-2.9620475485804487</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.4568148099960787</c:v>
+                  <c:v>-1.7930056336306706</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.7549126466105278</c:v>
+                  <c:v>-2.3413799644704358</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4216913545831105</c:v>
+                  <c:v>4.742625546582385</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.2352630892991865</c:v>
+                  <c:v>-2.0075984973084449</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.8692795334001531</c:v>
+                  <c:v>9.333353674828885</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3725470195343483</c:v>
+                  <c:v>2.570708236659776</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.48688608615028706</c:v>
+                  <c:v>-4.8462254027891838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.464469348912175</c:v>
+                  <c:v>2.5717899807409488</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.3344434387815713</c:v>
+                  <c:v>-9.0447708792058297</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.17238842880654204</c:v>
+                  <c:v>5.0938543900127939</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4220107422174273</c:v>
+                  <c:v>-5.6652526934797809</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.8313211790367916</c:v>
+                  <c:v>1.193065753965513</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.8655156333648719</c:v>
+                  <c:v>-8.7396015422229123</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7449628527101577</c:v>
+                  <c:v>-5.8504340646699493</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8983657636616886</c:v>
+                  <c:v>4.5563085794710005</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-5.0088238515256789</c:v>
+                  <c:v>-0.50986669413980401</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-6.6941104858112466</c:v>
+                  <c:v>-0.24261640966571107</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-8.8446258660020298</c:v>
+                  <c:v>7.9304074553934676</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-8.5624952762693809</c:v>
+                  <c:v>6.2014988414571981</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.1925021591615899</c:v>
+                  <c:v>-3.5243415840914105</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.45375608043095994</c:v>
+                  <c:v>6.0344773562181402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,100 +495,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>20.977236631190777</c:v>
+                  <c:v>19.287095128401528</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-11.852429198789526</c:v>
+                  <c:v>14.075412742881209</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-12.179965160619414</c:v>
+                  <c:v>-32.161609987503184</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3.6937639570102743</c:v>
+                  <c:v>-31.154679724682129</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>6.6765778781279295</c:v>
+                  <c:v>21.760077969314391</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.4097564257207154</c:v>
+                  <c:v>-32.912679749622882</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-33.622146813677574</c:v>
+                  <c:v>-18.240034448467611</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-16.133565074630493</c:v>
+                  <c:v>22.73421537962718</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>9.5587916459791309</c:v>
+                  <c:v>3.1532396669979903</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4059213769893724</c:v>
+                  <c:v>12.626112758847398</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.820461285519286</c:v>
+                  <c:v>-13.886142645741346</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>14.370444429988236</c:v>
+                  <c:v>-10.379016900892012</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.264737939831583</c:v>
+                  <c:v>-12.024139893411308</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>14.265074063749331</c:v>
+                  <c:v>9.227876639747155</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-17.705789267897558</c:v>
+                  <c:v>-11.022795491925335</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>18.607838600200459</c:v>
+                  <c:v>23.000061024486655</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>17.117641058603045</c:v>
+                  <c:v>2.712124709979328</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-6.4606582584508612</c:v>
+                  <c:v>-19.538676208367551</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-12.393408046736525</c:v>
+                  <c:v>2.7153699422228463</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>11.003330316344716</c:v>
+                  <c:v>-32.134312637617491</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-5.5171652864196261</c:v>
+                  <c:v>10.281563170038382</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.2660322266522819</c:v>
+                  <c:v>-21.995758080439344</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18.493963537110375</c:v>
+                  <c:v>-1.4208027381034611</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>15.596546900094616</c:v>
+                  <c:v>-31.218804626668735</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>3.2348885581304732</c:v>
+                  <c:v>-22.55130219400985</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.6950972909850659</c:v>
+                  <c:v>8.6689257384130016</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-20.026471554577036</c:v>
+                  <c:v>-6.529600082419412</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-25.082331457433739</c:v>
+                  <c:v>-5.7278492289971332</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-31.533877598006089</c:v>
+                  <c:v>18.791222366180403</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-30.687485828808143</c:v>
+                  <c:v>13.604496524371594</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.5775064774847696</c:v>
+                  <c:v>-15.573024752274232</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-3.6387317587071202</c:v>
+                  <c:v>13.103432068654421</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,100 +849,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>8.6590788770635925</c:v>
+                  <c:v>8.0956983761338428</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-2.2841430662631756</c:v>
+                  <c:v>6.3584709142937363</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-2.3933217202064716</c:v>
+                  <c:v>-9.0538699958343933</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>2.8979213190034248</c:v>
+                  <c:v>-8.7182265748940431</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>3.8921926260426432</c:v>
+                  <c:v>8.9200259897714638</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>2.1365854752402385</c:v>
+                  <c:v>-9.3042265832076261</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-9.5407156045591925</c:v>
+                  <c:v>-4.4133448161558704</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-3.7111883582101646</c:v>
+                  <c:v>9.2447384598757267</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>4.8529305486597103</c:v>
+                  <c:v>2.7177465556659968</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.4686404589964575</c:v>
+                  <c:v>5.8753709196157988</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>7.2734870951730954</c:v>
+                  <c:v>-2.9620475485804487</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6.4568148099960787</c:v>
+                  <c:v>-1.7930056336306706</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>8.7549126466105278</c:v>
+                  <c:v>-2.3413799644704358</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6.4216913545831105</c:v>
+                  <c:v>4.742625546582385</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-4.2352630892991865</c:v>
+                  <c:v>-2.0075984973084449</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>7.8692795334001531</c:v>
+                  <c:v>9.333353674828885</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>7.3725470195343483</c:v>
+                  <c:v>2.570708236659776</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.48688608615028706</c:v>
+                  <c:v>-4.8462254027891838</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-2.464469348912175</c:v>
+                  <c:v>2.5717899807409488</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>5.3344434387815713</c:v>
+                  <c:v>-9.0447708792058297</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>-0.17238842880654204</c:v>
+                  <c:v>5.0938543900127939</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.4220107422174273</c:v>
+                  <c:v>-5.6652526934797809</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>7.8313211790367916</c:v>
+                  <c:v>1.193065753965513</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.8655156333648719</c:v>
+                  <c:v>-8.7396015422229123</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>2.7449628527101577</c:v>
+                  <c:v>-5.8504340646699493</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>3.8983657636616886</c:v>
+                  <c:v>4.5563085794710005</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-5.0088238515256789</c:v>
+                  <c:v>-0.50986669413980401</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-6.6941104858112466</c:v>
+                  <c:v>-0.24261640966571107</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-8.8446258660020298</c:v>
+                  <c:v>7.9304074553934676</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-8.5624952762693809</c:v>
+                  <c:v>6.2014988414571981</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.1925021591615899</c:v>
+                  <c:v>-3.5243415840914105</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.45375608043095994</c:v>
+                  <c:v>6.0344773562181402</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,100 +954,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>26.098233089866206</c:v>
+                  <c:v>23.516836372566999</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>-4.4406431562717383</c:v>
+                  <c:v>9.7927900537197523</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-6.7197840831272853</c:v>
+                  <c:v>-39.964745723879041</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>5.0629258000806132</c:v>
+                  <c:v>-30.353108440276458</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>7.1398363884129132</c:v>
+                  <c:v>26.166626012538096</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.36237316351905768</c:v>
+                  <c:v>-37.422312604455122</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-26.830086708882241</c:v>
+                  <c:v>-18.035470189791202</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>-9.6931342909662224</c:v>
+                  <c:v>24.393674735037003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>5.3015410595750883</c:v>
+                  <c:v>-4.5894989460333768</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.7829670717939727</c:v>
+                  <c:v>15.703714798576476</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>16.967522288170429</c:v>
+                  <c:v>-7.5080423854717271</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.631790614940769</c:v>
+                  <c:v>-11.815063330453654</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>21.404662155770986</c:v>
+                  <c:v>-14.963211243563213</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>15.947435153992171</c:v>
+                  <c:v>2.2820824770814472</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-19.503609558803056</c:v>
+                  <c:v>-5.0683059129149015</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.503590786188436</c:v>
+                  <c:v>28.449406423645499</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.466312913114884</c:v>
+                  <c:v>3.0863791540935406</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-0.1253638195594462</c:v>
+                  <c:v>-25.640957704063428</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>-19.853455059597582</c:v>
+                  <c:v>7.7958445188613386</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>7.9977973057784144</c:v>
+                  <c:v>-26.250613886468429</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.16240902129444734</c:v>
+                  <c:v>8.1661960921313863</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>8.8716384069934957</c:v>
+                  <c:v>-21.992417135811777</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>16.584886855573863</c:v>
+                  <c:v>0.69834744053311582</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>7.6389032708564546</c:v>
+                  <c:v>-31.963842249024765</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.3589800872131814</c:v>
+                  <c:v>-17.519261579906498</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>7.7354206250785609</c:v>
+                  <c:v>9.8546287789354583</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-26.372431239146543</c:v>
+                  <c:v>-10.856846541179682</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-18.728556048011026</c:v>
+                  <c:v>-8.338762010397561</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>-24.810507019038031</c:v>
+                  <c:v>19.568059472444205</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>-38.556423042831128</c:v>
+                  <c:v>5.8368880554364218</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>0.56480865976764605</c:v>
+                  <c:v>-19.453280391876987</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>-5.574559983498748</c:v>
+                  <c:v>19.152451294974313</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2737,30 +2737,30 @@
       </c>
       <c r="C4">
         <f ca="1">RAND() * 20 - 10</f>
-        <v>8.6590788770635925</v>
+        <v>8.0956983761338428</v>
       </c>
       <c r="D4">
         <f ca="1">E4+(RAND() * 16-8)</f>
-        <v>26.098233089866206</v>
+        <v>23.516836372566999</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E17" ca="1" si="0">A4*C4+B4</f>
-        <v>20.977236631190777</v>
+        <v>19.287095128401528</v>
       </c>
       <c r="G4">
         <f ca="1">C4*C4</f>
-        <v>74.979646999208882</v>
+        <v>65.540332197336141</v>
       </c>
       <c r="H4">
         <f ca="1">C4*D4</f>
-        <v>225.98665887714256</v>
+        <v>190.38521403319595</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
       </c>
       <c r="L4">
         <f ca="1">SUM(C4:C35)</f>
-        <v>47.400528431652901</v>
+        <v>12.423332146340158</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2772,30 +2772,30 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C35" ca="1" si="1">RAND() * 20 - 10</f>
-        <v>-2.2841430662631756</v>
+        <v>6.3584709142937363</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D35" ca="1" si="2">E5+(RAND() * 16-8)</f>
-        <v>-4.4406431562717383</v>
+        <v>9.7927900537197523</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>-11.852429198789526</v>
+        <v>14.075412742881209</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G25" ca="1" si="3">C5*C5</f>
-        <v>5.2173095471581421</v>
+        <v>40.430152367919426</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H25" ca="1" si="4">C5*D5</f>
-        <v>10.143064275147115</v>
+        <v>62.267170726362039</v>
       </c>
       <c r="K5" t="s">
         <v>7</v>
       </c>
       <c r="L5">
         <f ca="1">SUM(G4:G35)</f>
-        <v>998.87940799696366</v>
+        <v>1167.8951544611627</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2807,30 +2807,30 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3933217202064716</v>
+        <v>-9.0538699958343933</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>-6.7197840831272853</v>
+        <v>-39.964745723879041</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.179965160619414</v>
+        <v>-32.161609987503184</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="3"/>
-        <v>5.7279888564120647</v>
+        <v>81.972561901470272</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="4"/>
-        <v>16.082605201246263</v>
+        <v>361.83561220057931</v>
       </c>
       <c r="K6" t="s">
         <v>8</v>
       </c>
       <c r="L6">
         <f ca="1">SUM(D4:D35)</f>
-        <v>16.375480708248539</v>
+        <v>-127.27181459499285</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2842,30 +2842,30 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>2.8979213190034248</v>
+        <v>-8.7182265748940431</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
-        <v>5.0629258000806132</v>
+        <v>-30.353108440276458</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>3.6937639570102743</v>
+        <v>-31.154679724682129</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="3"/>
-        <v>8.3979479711345491</v>
+        <v>76.007474611188712</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="4"/>
-        <v>14.67196061258608</v>
+        <v>264.62527663465892</v>
       </c>
       <c r="K7" t="s">
         <v>9</v>
       </c>
       <c r="L7">
         <f ca="1">SUM(H4:H35)</f>
-        <v>2696.1561155656991</v>
+        <v>3577.1130489389334</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2877,23 +2877,23 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8921926260426432</v>
+        <v>8.9200259897714638</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>7.1398363884129132</v>
+        <v>26.166626012538096</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>6.6765778781279295</v>
+        <v>21.760077969314391</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="3"/>
-        <v>15.149163438220727</v>
+        <v>79.566863658198386</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="4"/>
-        <v>27.789618542131677</v>
+        <v>233.40698409646987</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
@@ -2912,23 +2912,23 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>2.1365854752402385</v>
+        <v>-9.3042265832076261</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
-        <v>0.36237316351905768</v>
+        <v>-37.422312604455122</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>1.4097564257207154</v>
+        <v>-32.912679749622882</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="3"/>
-        <v>4.5649974930075556</v>
+        <v>86.568632311667457</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="4"/>
-        <v>0.77424123779167453</v>
+        <v>348.18567573947718</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2940,23 +2940,23 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.5407156045591925</v>
+        <v>-4.4133448161558704</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>-26.830086708882241</v>
+        <v>-18.035470189791202</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-33.622146813677574</v>
+        <v>-18.240034448467611</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>91.025254247079275</v>
+        <v>19.477612466289894</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="4"/>
-        <v>255.97822693510898</v>
+        <v>79.596748869048724</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2968,30 +2968,30 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.7111883582101646</v>
+        <v>9.2447384598757267</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="2"/>
-        <v>-9.6931342909662224</v>
+        <v>24.393674735037003</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>-16.133565074630493</v>
+        <v>22.73421537962718</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="3"/>
-        <v>13.772919030114657</v>
+        <v>85.465189191505431</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="4"/>
-        <v>35.973047135201583</v>
+        <v>225.51314300069541</v>
       </c>
       <c r="K11" t="s">
         <v>2</v>
       </c>
       <c r="L11">
         <f ca="1">(L8*L7-L4*L6)/(L8*L5-L4*L4)</f>
-        <v>2.8771355467091908</v>
+        <v>3.118055892613949</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3003,30 +3003,30 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>4.8529305486597103</v>
+        <v>2.7177465556659968</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>5.3015410595750883</v>
+        <v>-4.5894989460333768</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>9.5587916459791309</v>
+        <v>3.1532396669979903</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="3"/>
-        <v>23.550934910114638</v>
+        <v>7.3861463408343893</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="4"/>
-        <v>25.728010562985716</v>
+        <v>-12.473094952814932</v>
       </c>
       <c r="K12" t="s">
         <v>3</v>
       </c>
       <c r="L12">
         <f ca="1">(L6*L5-L7*L4)/(L8*L5-L4*L4)</f>
-        <v>-3.7500707679768648</v>
+        <v>-5.1877643312434092</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3038,23 +3038,23 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4686404589964575</v>
+        <v>5.8753709196157988</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>2.7829670717939727</v>
+        <v>15.703714798576476</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>2.4059213769893724</v>
+        <v>12.626112758847398</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="3"/>
-        <v>6.0941857157942403</v>
+        <v>34.519983443066998</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="4"/>
-        <v>6.8701451094854997</v>
+        <v>92.265149257496503</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3066,23 +3066,23 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>7.2734870951730954</v>
+        <v>-2.9620475485804487</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>16.967522288170429</v>
+        <v>-7.5080423854717271</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>16.820461285519286</v>
+        <v>-13.886142645741346</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="3"/>
-        <v>52.903614523649551</v>
+        <v>8.7737256800514452</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="4"/>
-        <v>123.41305440006948</v>
+        <v>22.239178542524634</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3094,23 +3094,23 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4568148099960787</v>
+        <v>-1.7930056336306706</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="2"/>
-        <v>20.631790614940769</v>
+        <v>-11.815063330453654</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>14.370444429988236</v>
+        <v>-10.379016900892012</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="3"/>
-        <v>41.690457490584699</v>
+        <v>3.2148692022313226</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="4"/>
-        <v>133.21565119928766</v>
+        <v>21.184475113206556</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3122,23 +3122,23 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>8.7549126466105278</v>
+        <v>-2.3413799644704358</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="2"/>
-        <v>21.404662155770986</v>
+        <v>-14.963211243563213</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>21.264737939831583</v>
+        <v>-12.024139893411308</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="3"/>
-        <v>76.648495449780953</v>
+        <v>5.4820601380235789</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="4"/>
-        <v>187.39594740398516</v>
+        <v>35.03456300981766</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3150,23 +3150,23 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>6.4216913545831105</v>
+        <v>4.742625546582385</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="2"/>
-        <v>15.947435153992171</v>
+        <v>2.2820824770814472</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>14.265074063749331</v>
+        <v>9.227876639747155</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="3"/>
-        <v>41.238119853527465</v>
+        <v>22.492497075095866</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="4"/>
-        <v>102.4095064561663</v>
+        <v>10.823062655214482</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3178,23 +3178,23 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.2352630892991865</v>
+        <v>-2.0075984973084449</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="2"/>
-        <v>-19.503609558803056</v>
+        <v>-5.0683059129149015</v>
       </c>
       <c r="E18">
         <f t="shared" ref="E18:E25" ca="1" si="5">A18*C18+B18</f>
-        <v>-17.705789267897558</v>
+        <v>-11.022795491925335</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="3"/>
-        <v>17.937453435580089</v>
+        <v>4.0304517263951256</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="4"/>
-        <v>82.602917672501377</v>
+        <v>10.175123334667463</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3206,23 +3206,23 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8692795334001531</v>
+        <v>9.333353674828885</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="2"/>
-        <v>15.503590786188436</v>
+        <v>28.449406423645499</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="5"/>
-        <v>18.607838600200459</v>
+        <v>23.000061024486655</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="3"/>
-        <v>61.925560374790528</v>
+        <v>87.111490819441855</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="4"/>
-        <v>122.00208966796384</v>
+        <v>265.52837199083223</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3234,23 +3234,23 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>7.3725470195343483</v>
+        <v>2.570708236659776</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="2"/>
-        <v>23.466312913114884</v>
+        <v>3.0863791540935406</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="5"/>
-        <v>17.117641058603045</v>
+        <v>2.712124709979328</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="3"/>
-        <v>54.354449555244805</v>
+        <v>6.6085408380304145</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="4"/>
-        <v>173.00649532704551</v>
+        <v>7.9341803128832966</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3262,23 +3262,23 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.48688608615028706</v>
+        <v>-4.8462254027891838</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="2"/>
-        <v>-0.1253638195594462</v>
+        <v>-25.640957704063428</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="5"/>
-        <v>-6.4606582584508612</v>
+        <v>-19.538676208367551</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="3"/>
-        <v>0.23705806088674475</v>
+        <v>23.485900654639188</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="4"/>
-        <v>6.1037899450149563E-2</v>
+        <v>124.26186057727521</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3290,23 +3290,23 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.464469348912175</v>
+        <v>2.5717899807409488</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="2"/>
-        <v>-19.853455059597582</v>
+        <v>7.7958445188613386</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="5"/>
-        <v>-12.393408046736525</v>
+        <v>2.7153699422228463</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="3"/>
-        <v>6.0736091717275995</v>
+        <v>6.6141037050395299</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="4"/>
-        <v>48.928231464383579</v>
+        <v>20.049274825021833</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3318,23 +3318,23 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>5.3344434387815713</v>
+        <v>-9.0447708792058297</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="2"/>
-        <v>7.9977973057784144</v>
+        <v>-26.250613886468429</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="5"/>
-        <v>11.003330316344716</v>
+        <v>-32.134312637617491</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="3"/>
-        <v>28.456286801559756</v>
+        <v>81.807880257329799</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="4"/>
-        <v>42.663797362514593</v>
+        <v>237.43078804160581</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3346,23 +3346,23 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.17238842880654204</v>
+        <v>5.0938543900127939</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>0.16240902129444734</v>
+        <v>8.1661960921313863</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="5"/>
-        <v>-5.5171652864196261</v>
+        <v>10.281563170038382</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="3"/>
-        <v>2.9717770386388214E-2</v>
+        <v>25.947352546652613</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="4"/>
-        <v>-2.7997436004958007E-2</v>
+        <v>41.597413813608782</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3374,23 +3374,23 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>2.4220107422174273</v>
+        <v>-5.6652526934797809</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>8.8716384069934957</v>
+        <v>-21.992417135811777</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="5"/>
-        <v>2.2660322266522819</v>
+        <v>-21.995758080439344</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="3"/>
-        <v>5.8661360354166128</v>
+        <v>32.095088080979913</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="4"/>
-        <v>21.487203522806951</v>
+        <v>124.59260041478856</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3402,23 +3402,23 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>7.8313211790367916</v>
+        <v>1.193065753965513</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>16.584886855573863</v>
+        <v>0.69834744053311582</v>
       </c>
       <c r="E26">
         <f t="shared" ref="E26:E35" ca="1" si="6">A26*C26+B26</f>
-        <v>18.493963537110375</v>
+        <v>-1.4208027381034611</v>
       </c>
       <c r="G26">
         <f t="shared" ref="G26:G35" ca="1" si="7">C26*C26</f>
-        <v>61.329591409230204</v>
+        <v>1.423405893285298</v>
       </c>
       <c r="H26">
         <f t="shared" ref="H26:H35" ca="1" si="8">C26*D26</f>
-        <v>129.88157568398449</v>
+        <v>0.83317441566952799</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3430,23 +3430,23 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>6.8655156333648719</v>
+        <v>-8.7396015422229123</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>7.6389032708564546</v>
+        <v>-31.963842249024765</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="6"/>
-        <v>15.596546900094616</v>
+        <v>-31.218804626668735</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="7"/>
-        <v>47.135304911977457</v>
+        <v>76.380635116825104</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="8"/>
-        <v>52.445009827827043</v>
+        <v>279.3512450149467</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3458,23 +3458,23 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7449628527101577</v>
+        <v>-5.8504340646699493</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>7.3589800872131814</v>
+        <v>-17.519261579906498</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="6"/>
-        <v>3.2348885581304732</v>
+        <v>-22.55130219400985</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="7"/>
-        <v>7.5348210627586871</v>
+        <v>34.227578745050543</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="8"/>
-        <v>20.200126973233939</v>
+        <v>102.49528473494846</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3486,23 +3486,23 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>3.8983657636616886</v>
+        <v>4.5563085794710005</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>7.7354206250785609</v>
+        <v>9.8546287789354583</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="6"/>
-        <v>6.6950972909850659</v>
+        <v>8.6689257384130016</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="7"/>
-        <v>15.19725562728958</v>
+        <v>20.759947871361046</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="8"/>
-        <v>30.155498932328761</v>
+        <v>44.90072965296546</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3514,23 +3514,23 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.0088238515256789</v>
+        <v>-0.50986669413980401</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>-26.372431239146543</v>
+        <v>-10.856846541179682</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="6"/>
-        <v>-20.026471554577036</v>
+        <v>-6.529600082419412</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="7"/>
-        <v>25.088316375612536</v>
+        <v>0.25996404579305243</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="8"/>
-        <v>132.09486261335812</v>
+        <v>5.5355444547344499</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3542,23 +3542,23 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>-6.6941104858112466</v>
+        <v>-0.24261640966571107</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>-18.728556048011026</v>
+        <v>-8.338762010397561</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="6"/>
-        <v>-25.082331457433739</v>
+        <v>-5.7278492289971332</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="7"/>
-        <v>44.811115196248082</v>
+        <v>5.8862722239080144E-2</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="8"/>
-        <v>125.37102342509425</v>
+        <v>2.0231205000194832</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3570,23 +3570,23 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.8446258660020298</v>
+        <v>7.9304074553934676</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="2"/>
-        <v>-24.810507019038031</v>
+        <v>19.568059472444205</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="6"/>
-        <v>-31.533877598006089</v>
+        <v>18.791222366180403</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="7"/>
-        <v>78.227406709552156</v>
+        <v>62.89136240856029</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="8"/>
-        <v>219.4396521292087</v>
+        <v>155.18268472785428</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3598,23 +3598,23 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.5624952762693809</v>
+        <v>6.2014988414571981</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="2"/>
-        <v>-38.556423042831128</v>
+        <v>5.8368880554364218</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="6"/>
-        <v>-30.687485828808143</v>
+        <v>13.604496524371594</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="7"/>
-        <v>73.316325356135465</v>
+        <v>38.458587880594969</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="8"/>
-        <v>330.13919017408546</v>
+        <v>36.197454513504326</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3626,23 +3626,23 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>3.1925021591615899</v>
+        <v>-3.5243415840914105</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="2"/>
-        <v>0.56480865976764605</v>
+        <v>-19.453280391876987</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="6"/>
-        <v>4.5775064774847696</v>
+        <v>-15.573024752274232</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="7"/>
-        <v>10.192070036251414</v>
+        <v>12.420983601355953</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="8"/>
-        <v>1.8031528658213738</v>
+        <v>68.560005032082117</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3654,23 +3654,23 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>0.45375608043095994</v>
+        <v>6.0344773562181402</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.574559983498748</v>
+        <v>19.152451294974313</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="6"/>
-        <v>-3.6387317587071202</v>
+        <v>13.103432068654421</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="7"/>
-        <v>0.20589458052806778</v>
+        <v>36.414916962709476</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="8"/>
-        <v>-2.5294904882396687</v>
+        <v>115.57503365559329</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
explain gradient and gradient descent
</commit_message>
<xml_diff>
--- a/sphinx-book/source/supervised/supervised/figures/linerexample.xlsx
+++ b/sphinx-book/source/supervised/supervised/figures/linerexample.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010"/>
+    <workbookView xWindow="240" yWindow="105" windowWidth="9360" windowHeight="3480"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -160,100 +160,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>8.0956983761338428</c:v>
+                  <c:v>-9.3236607823182176</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3584709142937363</c:v>
+                  <c:v>7.2284492158691442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.0538699958343933</c:v>
+                  <c:v>-9.5544621066152029</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.7182265748940431</c:v>
+                  <c:v>-6.9706693372283368</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9200259897714638</c:v>
+                  <c:v>-6.9100130587423862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-9.3042265832076261</c:v>
+                  <c:v>-1.5297141091051554</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-4.4133448161558704</c:v>
+                  <c:v>-4.4571853971175841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.2447384598757267</c:v>
+                  <c:v>-5.5087765266830075</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7177465556659968</c:v>
+                  <c:v>-6.4113212798241337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8753709196157988</c:v>
+                  <c:v>8.2194369936544547</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.9620475485804487</c:v>
+                  <c:v>-4.543543996614785</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.7930056336306706</c:v>
+                  <c:v>8.5727210354729451</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.3413799644704358</c:v>
+                  <c:v>2.6069786375610953</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.742625546582385</c:v>
+                  <c:v>2.0036628894437243</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.0075984973084449</c:v>
+                  <c:v>-2.219638733701002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.333353674828885</c:v>
+                  <c:v>2.568865786451461</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.570708236659776</c:v>
+                  <c:v>5.1515100092539825</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4.8462254027891838</c:v>
+                  <c:v>-3.9630714580795656</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5717899807409488</c:v>
+                  <c:v>6.7094181597368348</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-9.0447708792058297</c:v>
+                  <c:v>6.7155772910909448</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.0938543900127939</c:v>
+                  <c:v>-8.6889261123958477</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-5.6652526934797809</c:v>
+                  <c:v>-2.4356135117745836</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.193065753965513</c:v>
+                  <c:v>2.8823516890362058</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8.7396015422229123</c:v>
+                  <c:v>5.869794339984665</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-5.8504340646699493</c:v>
+                  <c:v>8.558082680191049</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5563085794710005</c:v>
+                  <c:v>3.6536566110692466</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.50986669413980401</c:v>
+                  <c:v>0.45377896356381697</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.24261640966571107</c:v>
+                  <c:v>9.7834398893335006</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.9304074553934676</c:v>
+                  <c:v>-1.4262116945963292</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.2014988414571981</c:v>
+                  <c:v>-9.2896050878444196</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-3.5243415840914105</c:v>
+                  <c:v>-9.5712704911017283</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.0344773562181402</c:v>
+                  <c:v>-6.7105313167625198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -265,100 +265,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>23.516836372566999</c:v>
+                  <c:v>-36.348931775224742</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7927900537197523</c:v>
+                  <c:v>16.826112139941365</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-39.964745723879041</c:v>
+                  <c:v>-30.957989999402947</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-30.353108440276458</c:v>
+                  <c:v>-31.3787302226532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.166626012538096</c:v>
+                  <c:v>-25.992647104177941</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-37.422312604455122</c:v>
+                  <c:v>-4.4206129949796829</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.035470189791202</c:v>
+                  <c:v>-17.516098221240696</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.393674735037003</c:v>
+                  <c:v>-14.596332354918925</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.5894989460333768</c:v>
+                  <c:v>-28.133025936301003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.703714798576476</c:v>
+                  <c:v>18.451254976629549</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7.5080423854717271</c:v>
+                  <c:v>-22.058232018014749</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-11.815063330453654</c:v>
+                  <c:v>14.380137150126686</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-14.963211243563213</c:v>
+                  <c:v>6.9842940846947776</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2820824770814472</c:v>
+                  <c:v>5.7279111182969586</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-5.0683059129149015</c:v>
+                  <c:v>-11.623975004795764</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.449406423645499</c:v>
+                  <c:v>2.538072058131231</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0863791540935406</c:v>
+                  <c:v>5.169051944279639</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-25.640957704063428</c:v>
+                  <c:v>-17.982244303582014</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.7958445188613386</c:v>
+                  <c:v>15.240506987323121</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-26.250613886468429</c:v>
+                  <c:v>15.178482676057291</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.1661960921313863</c:v>
+                  <c:v>-35.90249646870852</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-21.992417135811777</c:v>
+                  <c:v>-9.0881344948484024</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.69834744053311582</c:v>
+                  <c:v>7.5563269610367367</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-31.963842249024765</c:v>
+                  <c:v>5.3021711998670007</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-17.519261579906498</c:v>
+                  <c:v>22.612292848383756</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.8546287789354583</c:v>
+                  <c:v>12.089442264706967</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-10.856846541179682</c:v>
+                  <c:v>-7.4443975621264489</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-8.338762010397561</c:v>
+                  <c:v>26.715761935747508</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>19.568059472444205</c:v>
+                  <c:v>-10.116711522812965</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.8368880554364218</c:v>
+                  <c:v>-37.228751217942261</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-19.453280391876987</c:v>
+                  <c:v>-41.364246226299151</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>19.152451294974313</c:v>
+                  <c:v>-23.218327756788241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -390,100 +390,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>8.0956983761338428</c:v>
+                  <c:v>-9.3236607823182176</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3584709142937363</c:v>
+                  <c:v>7.2284492158691442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.0538699958343933</c:v>
+                  <c:v>-9.5544621066152029</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.7182265748940431</c:v>
+                  <c:v>-6.9706693372283368</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9200259897714638</c:v>
+                  <c:v>-6.9100130587423862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-9.3042265832076261</c:v>
+                  <c:v>-1.5297141091051554</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-4.4133448161558704</c:v>
+                  <c:v>-4.4571853971175841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.2447384598757267</c:v>
+                  <c:v>-5.5087765266830075</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7177465556659968</c:v>
+                  <c:v>-6.4113212798241337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8753709196157988</c:v>
+                  <c:v>8.2194369936544547</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.9620475485804487</c:v>
+                  <c:v>-4.543543996614785</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.7930056336306706</c:v>
+                  <c:v>8.5727210354729451</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.3413799644704358</c:v>
+                  <c:v>2.6069786375610953</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.742625546582385</c:v>
+                  <c:v>2.0036628894437243</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.0075984973084449</c:v>
+                  <c:v>-2.219638733701002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.333353674828885</c:v>
+                  <c:v>2.568865786451461</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.570708236659776</c:v>
+                  <c:v>5.1515100092539825</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4.8462254027891838</c:v>
+                  <c:v>-3.9630714580795656</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5717899807409488</c:v>
+                  <c:v>6.7094181597368348</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-9.0447708792058297</c:v>
+                  <c:v>6.7155772910909448</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.0938543900127939</c:v>
+                  <c:v>-8.6889261123958477</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-5.6652526934797809</c:v>
+                  <c:v>-2.4356135117745836</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.193065753965513</c:v>
+                  <c:v>2.8823516890362058</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8.7396015422229123</c:v>
+                  <c:v>5.869794339984665</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-5.8504340646699493</c:v>
+                  <c:v>8.558082680191049</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5563085794710005</c:v>
+                  <c:v>3.6536566110692466</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.50986669413980401</c:v>
+                  <c:v>0.45377896356381697</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.24261640966571107</c:v>
+                  <c:v>9.7834398893335006</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.9304074553934676</c:v>
+                  <c:v>-1.4262116945963292</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.2014988414571981</c:v>
+                  <c:v>-9.2896050878444196</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-3.5243415840914105</c:v>
+                  <c:v>-9.5712704911017283</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.0344773562181402</c:v>
+                  <c:v>-6.7105313167625198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -495,100 +495,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>19.287095128401528</c:v>
+                  <c:v>-32.970982346954656</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>14.075412742881209</c:v>
+                  <c:v>16.685347647607433</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-32.161609987503184</c:v>
+                  <c:v>-33.663386319845607</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-31.154679724682129</c:v>
+                  <c:v>-25.91200801168501</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.760077969314391</c:v>
+                  <c:v>-25.730039176227159</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-32.912679749622882</c:v>
+                  <c:v>-9.5891423273154661</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.240034448467611</c:v>
+                  <c:v>-18.371556191352752</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>22.73421537962718</c:v>
+                  <c:v>-21.526329580049023</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3.1532396669979903</c:v>
+                  <c:v>-24.233963839472402</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>12.626112758847398</c:v>
+                  <c:v>19.658310980963364</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-13.886142645741346</c:v>
+                  <c:v>-18.630631989844353</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-10.379016900892012</c:v>
+                  <c:v>20.718163106418835</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-12.024139893411308</c:v>
+                  <c:v>2.8209359126832858</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.227876639747155</c:v>
+                  <c:v>1.0109886683311728</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-11.022795491925335</c:v>
+                  <c:v>-11.658916201103006</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.000061024486655</c:v>
+                  <c:v>2.7065973593543831</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.712124709979328</c:v>
+                  <c:v>10.454530027761948</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-19.538676208367551</c:v>
+                  <c:v>-16.889214374238698</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.7153699422228463</c:v>
+                  <c:v>15.128254479210504</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-32.134312637617491</c:v>
+                  <c:v>15.146731873272834</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>10.281563170038382</c:v>
+                  <c:v>-31.066778337187543</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-21.995758080439344</c:v>
+                  <c:v>-12.306840535323751</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>-1.4208027381034611</c:v>
+                  <c:v>3.6470550671086173</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-31.218804626668735</c:v>
+                  <c:v>12.609383019953995</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-22.55130219400985</c:v>
+                  <c:v>20.674248040573147</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>8.6689257384130016</c:v>
+                  <c:v>5.9609698332077397</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-6.529600082419412</c:v>
+                  <c:v>-3.6386631093085491</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-5.7278492289971332</c:v>
+                  <c:v>24.350319668000502</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>18.791222366180403</c:v>
+                  <c:v>-9.2786350837889877</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>13.604496524371594</c:v>
+                  <c:v>-32.868815263533257</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-15.573024752274232</c:v>
+                  <c:v>-33.713811473305185</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.103432068654421</c:v>
+                  <c:v>-25.131593950287559</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -849,100 +849,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>8.0956983761338428</c:v>
+                  <c:v>-9.3236607823182176</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6.3584709142937363</c:v>
+                  <c:v>7.2284492158691442</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-9.0538699958343933</c:v>
+                  <c:v>-9.5544621066152029</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-8.7182265748940431</c:v>
+                  <c:v>-6.9706693372283368</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>8.9200259897714638</c:v>
+                  <c:v>-6.9100130587423862</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-9.3042265832076261</c:v>
+                  <c:v>-1.5297141091051554</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-4.4133448161558704</c:v>
+                  <c:v>-4.4571853971175841</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>9.2447384598757267</c:v>
+                  <c:v>-5.5087765266830075</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>2.7177465556659968</c:v>
+                  <c:v>-6.4113212798241337</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>5.8753709196157988</c:v>
+                  <c:v>8.2194369936544547</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-2.9620475485804487</c:v>
+                  <c:v>-4.543543996614785</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-1.7930056336306706</c:v>
+                  <c:v>8.5727210354729451</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-2.3413799644704358</c:v>
+                  <c:v>2.6069786375610953</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>4.742625546582385</c:v>
+                  <c:v>2.0036628894437243</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-2.0075984973084449</c:v>
+                  <c:v>-2.219638733701002</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>9.333353674828885</c:v>
+                  <c:v>2.568865786451461</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>2.570708236659776</c:v>
+                  <c:v>5.1515100092539825</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-4.8462254027891838</c:v>
+                  <c:v>-3.9630714580795656</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.5717899807409488</c:v>
+                  <c:v>6.7094181597368348</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-9.0447708792058297</c:v>
+                  <c:v>6.7155772910909448</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>5.0938543900127939</c:v>
+                  <c:v>-8.6889261123958477</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-5.6652526934797809</c:v>
+                  <c:v>-2.4356135117745836</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>1.193065753965513</c:v>
+                  <c:v>2.8823516890362058</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-8.7396015422229123</c:v>
+                  <c:v>5.869794339984665</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-5.8504340646699493</c:v>
+                  <c:v>8.558082680191049</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>4.5563085794710005</c:v>
+                  <c:v>3.6536566110692466</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-0.50986669413980401</c:v>
+                  <c:v>0.45377896356381697</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-0.24261640966571107</c:v>
+                  <c:v>9.7834398893335006</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>7.9304074553934676</c:v>
+                  <c:v>-1.4262116945963292</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.2014988414571981</c:v>
+                  <c:v>-9.2896050878444196</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-3.5243415840914105</c:v>
+                  <c:v>-9.5712704911017283</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>6.0344773562181402</c:v>
+                  <c:v>-6.7105313167625198</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -954,100 +954,100 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="32"/>
                 <c:pt idx="0">
-                  <c:v>23.516836372566999</c:v>
+                  <c:v>-36.348931775224742</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.7927900537197523</c:v>
+                  <c:v>16.826112139941365</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>-39.964745723879041</c:v>
+                  <c:v>-30.957989999402947</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>-30.353108440276458</c:v>
+                  <c:v>-31.3787302226532</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>26.166626012538096</c:v>
+                  <c:v>-25.992647104177941</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>-37.422312604455122</c:v>
+                  <c:v>-4.4206129949796829</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>-18.035470189791202</c:v>
+                  <c:v>-17.516098221240696</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.393674735037003</c:v>
+                  <c:v>-14.596332354918925</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>-4.5894989460333768</c:v>
+                  <c:v>-28.133025936301003</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>15.703714798576476</c:v>
+                  <c:v>18.451254976629549</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>-7.5080423854717271</c:v>
+                  <c:v>-22.058232018014749</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>-11.815063330453654</c:v>
+                  <c:v>14.380137150126686</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>-14.963211243563213</c:v>
+                  <c:v>6.9842940846947776</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>2.2820824770814472</c:v>
+                  <c:v>5.7279111182969586</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>-5.0683059129149015</c:v>
+                  <c:v>-11.623975004795764</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>28.449406423645499</c:v>
+                  <c:v>2.538072058131231</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>3.0863791540935406</c:v>
+                  <c:v>5.169051944279639</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>-25.640957704063428</c:v>
+                  <c:v>-17.982244303582014</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>7.7958445188613386</c:v>
+                  <c:v>15.240506987323121</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>-26.250613886468429</c:v>
+                  <c:v>15.178482676057291</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.1661960921313863</c:v>
+                  <c:v>-35.90249646870852</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>-21.992417135811777</c:v>
+                  <c:v>-9.0881344948484024</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.69834744053311582</c:v>
+                  <c:v>7.5563269610367367</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>-31.963842249024765</c:v>
+                  <c:v>5.3021711998670007</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>-17.519261579906498</c:v>
+                  <c:v>22.612292848383756</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>9.8546287789354583</c:v>
+                  <c:v>12.089442264706967</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>-10.856846541179682</c:v>
+                  <c:v>-7.4443975621264489</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>-8.338762010397561</c:v>
+                  <c:v>26.715761935747508</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>19.568059472444205</c:v>
+                  <c:v>-10.116711522812965</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>5.8368880554364218</c:v>
+                  <c:v>-37.228751217942261</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>-19.453280391876987</c:v>
+                  <c:v>-41.364246226299151</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>19.152451294974313</c:v>
+                  <c:v>-23.218327756788241</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2695,7 +2695,7 @@
   <dimension ref="A1:L35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="K20" sqref="K20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2737,30 +2737,30 @@
       </c>
       <c r="C4">
         <f ca="1">RAND() * 20 - 10</f>
-        <v>8.0956983761338428</v>
+        <v>-9.3236607823182176</v>
       </c>
       <c r="D4">
         <f ca="1">E4+(RAND() * 16-8)</f>
-        <v>23.516836372566999</v>
+        <v>-36.348931775224742</v>
       </c>
       <c r="E4">
         <f t="shared" ref="E4:E17" ca="1" si="0">A4*C4+B4</f>
-        <v>19.287095128401528</v>
+        <v>-32.970982346954656</v>
       </c>
       <c r="G4">
         <f ca="1">C4*C4</f>
-        <v>65.540332197336141</v>
+        <v>86.930650383738751</v>
       </c>
       <c r="H4">
         <f ca="1">C4*D4</f>
-        <v>190.38521403319595</v>
+        <v>338.90510967182342</v>
       </c>
       <c r="K4" t="s">
         <v>6</v>
       </c>
       <c r="L4">
         <f ca="1">SUM(C4:C35)</f>
-        <v>12.423332146340158</v>
+        <v>-18.53649080879174</v>
       </c>
     </row>
     <row r="5" spans="1:12" x14ac:dyDescent="0.25">
@@ -2772,30 +2772,30 @@
       </c>
       <c r="C5">
         <f t="shared" ref="C5:C35" ca="1" si="1">RAND() * 20 - 10</f>
-        <v>6.3584709142937363</v>
+        <v>7.2284492158691442</v>
       </c>
       <c r="D5">
         <f t="shared" ref="D5:D35" ca="1" si="2">E5+(RAND() * 16-8)</f>
-        <v>9.7927900537197523</v>
+        <v>16.826112139941365</v>
       </c>
       <c r="E5">
         <f t="shared" ca="1" si="0"/>
-        <v>14.075412742881209</v>
+        <v>16.685347647607433</v>
       </c>
       <c r="G5">
         <f t="shared" ref="G5:G25" ca="1" si="3">C5*C5</f>
-        <v>40.430152367919426</v>
+        <v>52.250478066399246</v>
       </c>
       <c r="H5">
         <f t="shared" ref="H5:H25" ca="1" si="4">C5*D5</f>
-        <v>62.267170726362039</v>
+        <v>121.62669710408545</v>
       </c>
       <c r="K5" t="s">
         <v>7</v>
       </c>
       <c r="L5">
         <f ca="1">SUM(G4:G35)</f>
-        <v>1167.8951544611627</v>
+        <v>1268.5311622259285</v>
       </c>
     </row>
     <row r="6" spans="1:12" x14ac:dyDescent="0.25">
@@ -2807,30 +2807,30 @@
       </c>
       <c r="C6">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.0538699958343933</v>
+        <v>-9.5544621066152029</v>
       </c>
       <c r="D6">
         <f t="shared" ca="1" si="2"/>
-        <v>-39.964745723879041</v>
+        <v>-30.957989999402947</v>
       </c>
       <c r="E6">
         <f t="shared" ca="1" si="0"/>
-        <v>-32.161609987503184</v>
+        <v>-33.663386319845607</v>
       </c>
       <c r="G6">
         <f t="shared" ca="1" si="3"/>
-        <v>81.972561901470272</v>
+        <v>91.287746146745818</v>
       </c>
       <c r="H6">
         <f t="shared" ca="1" si="4"/>
-        <v>361.83561220057931</v>
+        <v>295.78694234626789</v>
       </c>
       <c r="K6" t="s">
         <v>8</v>
       </c>
       <c r="L6">
         <f ca="1">SUM(D4:D35)</f>
-        <v>-127.27181459499285</v>
+        <v>-230.60006683959506</v>
       </c>
     </row>
     <row r="7" spans="1:12" x14ac:dyDescent="0.25">
@@ -2842,30 +2842,30 @@
       </c>
       <c r="C7">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.7182265748940431</v>
+        <v>-6.9706693372283368</v>
       </c>
       <c r="D7">
         <f t="shared" ca="1" si="2"/>
-        <v>-30.353108440276458</v>
+        <v>-31.3787302226532</v>
       </c>
       <c r="E7">
         <f t="shared" ca="1" si="0"/>
-        <v>-31.154679724682129</v>
+        <v>-25.91200801168501</v>
       </c>
       <c r="G7">
         <f t="shared" ca="1" si="3"/>
-        <v>76.007474611188712</v>
+        <v>48.590231008975337</v>
       </c>
       <c r="H7">
         <f t="shared" ca="1" si="4"/>
-        <v>264.62527663465892</v>
+        <v>218.73075260420876</v>
       </c>
       <c r="K7" t="s">
         <v>9</v>
       </c>
       <c r="L7">
         <f ca="1">SUM(H4:H35)</f>
-        <v>3577.1130489389334</v>
+        <v>4034.1753591963957</v>
       </c>
     </row>
     <row r="8" spans="1:12" x14ac:dyDescent="0.25">
@@ -2877,23 +2877,23 @@
       </c>
       <c r="C8">
         <f t="shared" ca="1" si="1"/>
-        <v>8.9200259897714638</v>
+        <v>-6.9100130587423862</v>
       </c>
       <c r="D8">
         <f t="shared" ca="1" si="2"/>
-        <v>26.166626012538096</v>
+        <v>-25.992647104177941</v>
       </c>
       <c r="E8">
         <f t="shared" ca="1" si="0"/>
-        <v>21.760077969314391</v>
+        <v>-25.730039176227159</v>
       </c>
       <c r="G8">
         <f t="shared" ca="1" si="3"/>
-        <v>79.566863658198386</v>
+        <v>47.748280471990306</v>
       </c>
       <c r="H8">
         <f t="shared" ca="1" si="4"/>
-        <v>233.40698409646987</v>
+        <v>179.60953092115204</v>
       </c>
       <c r="K8" t="s">
         <v>10</v>
@@ -2912,23 +2912,23 @@
       </c>
       <c r="C9">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.3042265832076261</v>
+        <v>-1.5297141091051554</v>
       </c>
       <c r="D9">
         <f t="shared" ca="1" si="2"/>
-        <v>-37.422312604455122</v>
+        <v>-4.4206129949796829</v>
       </c>
       <c r="E9">
         <f t="shared" ca="1" si="0"/>
-        <v>-32.912679749622882</v>
+        <v>-9.5891423273154661</v>
       </c>
       <c r="G9">
         <f t="shared" ca="1" si="3"/>
-        <v>86.568632311667457</v>
+        <v>2.3400252555953793</v>
       </c>
       <c r="H9">
         <f t="shared" ca="1" si="4"/>
-        <v>348.18567573947718</v>
+        <v>6.7622740693140182</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.25">
@@ -2940,23 +2940,23 @@
       </c>
       <c r="C10">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.4133448161558704</v>
+        <v>-4.4571853971175841</v>
       </c>
       <c r="D10">
         <f t="shared" ca="1" si="2"/>
-        <v>-18.035470189791202</v>
+        <v>-17.516098221240696</v>
       </c>
       <c r="E10">
         <f t="shared" ca="1" si="0"/>
-        <v>-18.240034448467611</v>
+        <v>-18.371556191352752</v>
       </c>
       <c r="G10">
         <f t="shared" ca="1" si="3"/>
-        <v>19.477612466289894</v>
+        <v>19.866501664278235</v>
       </c>
       <c r="H10">
         <f t="shared" ca="1" si="4"/>
-        <v>79.596748869048724</v>
+        <v>78.072497206191315</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.25">
@@ -2968,30 +2968,30 @@
       </c>
       <c r="C11">
         <f t="shared" ca="1" si="1"/>
-        <v>9.2447384598757267</v>
+        <v>-5.5087765266830075</v>
       </c>
       <c r="D11">
         <f t="shared" ca="1" si="2"/>
-        <v>24.393674735037003</v>
+        <v>-14.596332354918925</v>
       </c>
       <c r="E11">
         <f t="shared" ca="1" si="0"/>
-        <v>22.73421537962718</v>
+        <v>-21.526329580049023</v>
       </c>
       <c r="G11">
         <f t="shared" ca="1" si="3"/>
-        <v>85.465189191505431</v>
+        <v>30.346618820933699</v>
       </c>
       <c r="H11">
         <f t="shared" ca="1" si="4"/>
-        <v>225.51314300069541</v>
+        <v>80.407933052441081</v>
       </c>
       <c r="K11" t="s">
         <v>2</v>
       </c>
       <c r="L11">
         <f ca="1">(L8*L7-L4*L6)/(L8*L5-L4*L4)</f>
-        <v>3.118055892613949</v>
+        <v>3.1011420992752359</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.25">
@@ -3003,30 +3003,30 @@
       </c>
       <c r="C12">
         <f t="shared" ca="1" si="1"/>
-        <v>2.7177465556659968</v>
+        <v>-6.4113212798241337</v>
       </c>
       <c r="D12">
         <f t="shared" ca="1" si="2"/>
-        <v>-4.5894989460333768</v>
+        <v>-28.133025936301003</v>
       </c>
       <c r="E12">
         <f t="shared" ca="1" si="0"/>
-        <v>3.1532396669979903</v>
+        <v>-24.233963839472402</v>
       </c>
       <c r="G12">
         <f t="shared" ca="1" si="3"/>
-        <v>7.3861463408343893</v>
+        <v>41.105040553125768</v>
       </c>
       <c r="H12">
         <f t="shared" ca="1" si="4"/>
-        <v>-12.473094952814932</v>
+        <v>180.36986785125089</v>
       </c>
       <c r="K12" t="s">
         <v>3</v>
       </c>
       <c r="L12">
         <f ca="1">(L6*L5-L7*L4)/(L8*L5-L4*L4)</f>
-        <v>-5.1877643312434092</v>
+        <v>-5.4098679631132045</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.25">
@@ -3038,23 +3038,23 @@
       </c>
       <c r="C13">
         <f t="shared" ca="1" si="1"/>
-        <v>5.8753709196157988</v>
+        <v>8.2194369936544547</v>
       </c>
       <c r="D13">
         <f t="shared" ca="1" si="2"/>
-        <v>15.703714798576476</v>
+        <v>18.451254976629549</v>
       </c>
       <c r="E13">
         <f t="shared" ca="1" si="0"/>
-        <v>12.626112758847398</v>
+        <v>19.658310980963364</v>
       </c>
       <c r="G13">
         <f t="shared" ca="1" si="3"/>
-        <v>34.519983443066998</v>
+        <v>67.559144492655378</v>
       </c>
       <c r="H13">
         <f t="shared" ca="1" si="4"/>
-        <v>92.265149257496503</v>
+        <v>151.65892773425978</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.25">
@@ -3066,23 +3066,23 @@
       </c>
       <c r="C14">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.9620475485804487</v>
+        <v>-4.543543996614785</v>
       </c>
       <c r="D14">
         <f t="shared" ca="1" si="2"/>
-        <v>-7.5080423854717271</v>
+        <v>-22.058232018014749</v>
       </c>
       <c r="E14">
         <f t="shared" ca="1" si="0"/>
-        <v>-13.886142645741346</v>
+        <v>-18.630631989844353</v>
       </c>
       <c r="G14">
         <f t="shared" ca="1" si="3"/>
-        <v>8.7737256800514452</v>
+        <v>20.643792049174255</v>
       </c>
       <c r="H14">
         <f t="shared" ca="1" si="4"/>
-        <v>22.239178542524634</v>
+        <v>100.22254766138695</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.25">
@@ -3094,23 +3094,23 @@
       </c>
       <c r="C15">
         <f t="shared" ca="1" si="1"/>
-        <v>-1.7930056336306706</v>
+        <v>8.5727210354729451</v>
       </c>
       <c r="D15">
         <f t="shared" ca="1" si="2"/>
-        <v>-11.815063330453654</v>
+        <v>14.380137150126686</v>
       </c>
       <c r="E15">
         <f t="shared" ca="1" si="0"/>
-        <v>-10.379016900892012</v>
+        <v>20.718163106418835</v>
       </c>
       <c r="G15">
         <f t="shared" ca="1" si="3"/>
-        <v>3.2148692022313226</v>
+        <v>73.491545952040326</v>
       </c>
       <c r="H15">
         <f t="shared" ca="1" si="4"/>
-        <v>21.184475113206556</v>
+        <v>123.27690423987701</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.25">
@@ -3122,23 +3122,23 @@
       </c>
       <c r="C16">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.3413799644704358</v>
+        <v>2.6069786375610953</v>
       </c>
       <c r="D16">
         <f t="shared" ca="1" si="2"/>
-        <v>-14.963211243563213</v>
+        <v>6.9842940846947776</v>
       </c>
       <c r="E16">
         <f t="shared" ca="1" si="0"/>
-        <v>-12.024139893411308</v>
+        <v>2.8209359126832858</v>
       </c>
       <c r="G16">
         <f t="shared" ca="1" si="3"/>
-        <v>5.4820601380235789</v>
+        <v>6.7963376166999048</v>
       </c>
       <c r="H16">
         <f t="shared" ca="1" si="4"/>
-        <v>35.03456300981766</v>
+        <v>18.207905477243607</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -3150,23 +3150,23 @@
       </c>
       <c r="C17">
         <f t="shared" ca="1" si="1"/>
-        <v>4.742625546582385</v>
+        <v>2.0036628894437243</v>
       </c>
       <c r="D17">
         <f t="shared" ca="1" si="2"/>
-        <v>2.2820824770814472</v>
+        <v>5.7279111182969586</v>
       </c>
       <c r="E17">
         <f t="shared" ca="1" si="0"/>
-        <v>9.227876639747155</v>
+        <v>1.0109886683311728</v>
       </c>
       <c r="G17">
         <f t="shared" ca="1" si="3"/>
-        <v>22.492497075095866</v>
+        <v>4.0146649745339742</v>
       </c>
       <c r="H17">
         <f t="shared" ca="1" si="4"/>
-        <v>10.823062655214482</v>
+        <v>11.476802941763719</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
@@ -3178,23 +3178,23 @@
       </c>
       <c r="C18">
         <f t="shared" ca="1" si="1"/>
-        <v>-2.0075984973084449</v>
+        <v>-2.219638733701002</v>
       </c>
       <c r="D18">
         <f t="shared" ca="1" si="2"/>
-        <v>-5.0683059129149015</v>
+        <v>-11.623975004795764</v>
       </c>
       <c r="E18">
         <f t="shared" ref="E18:E25" ca="1" si="5">A18*C18+B18</f>
-        <v>-11.022795491925335</v>
+        <v>-11.658916201103006</v>
       </c>
       <c r="G18">
         <f t="shared" ca="1" si="3"/>
-        <v>4.0304517263951256</v>
+        <v>4.9267961081457878</v>
       </c>
       <c r="H18">
         <f t="shared" ca="1" si="4"/>
-        <v>10.175123334667463</v>
+        <v>25.801025160216966</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
@@ -3206,23 +3206,23 @@
       </c>
       <c r="C19">
         <f t="shared" ca="1" si="1"/>
-        <v>9.333353674828885</v>
+        <v>2.568865786451461</v>
       </c>
       <c r="D19">
         <f t="shared" ca="1" si="2"/>
-        <v>28.449406423645499</v>
+        <v>2.538072058131231</v>
       </c>
       <c r="E19">
         <f t="shared" ca="1" si="5"/>
-        <v>23.000061024486655</v>
+        <v>2.7065973593543831</v>
       </c>
       <c r="G19">
         <f t="shared" ca="1" si="3"/>
-        <v>87.111490819441855</v>
+        <v>6.5990714288008832</v>
       </c>
       <c r="H19">
         <f t="shared" ca="1" si="4"/>
-        <v>265.52837199083223</v>
+        <v>6.5199664736817633</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.25">
@@ -3234,23 +3234,23 @@
       </c>
       <c r="C20">
         <f t="shared" ca="1" si="1"/>
-        <v>2.570708236659776</v>
+        <v>5.1515100092539825</v>
       </c>
       <c r="D20">
         <f t="shared" ca="1" si="2"/>
-        <v>3.0863791540935406</v>
+        <v>5.169051944279639</v>
       </c>
       <c r="E20">
         <f t="shared" ca="1" si="5"/>
-        <v>2.712124709979328</v>
+        <v>10.454530027761948</v>
       </c>
       <c r="G20">
         <f t="shared" ca="1" si="3"/>
-        <v>6.6085408380304145</v>
+        <v>26.538055375443967</v>
       </c>
       <c r="H20">
         <f t="shared" ca="1" si="4"/>
-        <v>7.9341803128832966</v>
+        <v>26.62842282931032</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.25">
@@ -3262,23 +3262,23 @@
       </c>
       <c r="C21">
         <f t="shared" ca="1" si="1"/>
-        <v>-4.8462254027891838</v>
+        <v>-3.9630714580795656</v>
       </c>
       <c r="D21">
         <f t="shared" ca="1" si="2"/>
-        <v>-25.640957704063428</v>
+        <v>-17.982244303582014</v>
       </c>
       <c r="E21">
         <f t="shared" ca="1" si="5"/>
-        <v>-19.538676208367551</v>
+        <v>-16.889214374238698</v>
       </c>
       <c r="G21">
         <f t="shared" ca="1" si="3"/>
-        <v>23.485900654639188</v>
+        <v>15.705935381844894</v>
       </c>
       <c r="H21">
         <f t="shared" ca="1" si="4"/>
-        <v>124.26186057727521</v>
+        <v>71.264919151739733</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
@@ -3290,23 +3290,23 @@
       </c>
       <c r="C22">
         <f t="shared" ca="1" si="1"/>
-        <v>2.5717899807409488</v>
+        <v>6.7094181597368348</v>
       </c>
       <c r="D22">
         <f t="shared" ca="1" si="2"/>
-        <v>7.7958445188613386</v>
+        <v>15.240506987323121</v>
       </c>
       <c r="E22">
         <f t="shared" ca="1" si="5"/>
-        <v>2.7153699422228463</v>
+        <v>15.128254479210504</v>
       </c>
       <c r="G22">
         <f t="shared" ca="1" si="3"/>
-        <v>6.6141037050395299</v>
+        <v>45.016292042206416</v>
       </c>
       <c r="H22">
         <f t="shared" ca="1" si="4"/>
-        <v>20.049274825021833</v>
+        <v>102.25493434434186</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
@@ -3318,23 +3318,23 @@
       </c>
       <c r="C23">
         <f t="shared" ca="1" si="1"/>
-        <v>-9.0447708792058297</v>
+        <v>6.7155772910909448</v>
       </c>
       <c r="D23">
         <f t="shared" ca="1" si="2"/>
-        <v>-26.250613886468429</v>
+        <v>15.178482676057291</v>
       </c>
       <c r="E23">
         <f t="shared" ca="1" si="5"/>
-        <v>-32.134312637617491</v>
+        <v>15.146731873272834</v>
       </c>
       <c r="G23">
         <f t="shared" ca="1" si="3"/>
-        <v>81.807880257329799</v>
+        <v>45.098978352616392</v>
       </c>
       <c r="H23">
         <f t="shared" ca="1" si="4"/>
-        <v>237.43078804160581</v>
+        <v>101.93227357254766</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.25">
@@ -3346,23 +3346,23 @@
       </c>
       <c r="C24">
         <f t="shared" ca="1" si="1"/>
-        <v>5.0938543900127939</v>
+        <v>-8.6889261123958477</v>
       </c>
       <c r="D24">
         <f t="shared" ca="1" si="2"/>
-        <v>8.1661960921313863</v>
+        <v>-35.90249646870852</v>
       </c>
       <c r="E24">
         <f t="shared" ca="1" si="5"/>
-        <v>10.281563170038382</v>
+        <v>-31.066778337187543</v>
       </c>
       <c r="G24">
         <f t="shared" ca="1" si="3"/>
-        <v>25.947352546652613</v>
+        <v>75.497436986674415</v>
       </c>
       <c r="H24">
         <f t="shared" ca="1" si="4"/>
-        <v>41.597413813608782</v>
+        <v>311.95413906716118</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
@@ -3374,23 +3374,23 @@
       </c>
       <c r="C25">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.6652526934797809</v>
+        <v>-2.4356135117745836</v>
       </c>
       <c r="D25">
         <f t="shared" ca="1" si="2"/>
-        <v>-21.992417135811777</v>
+        <v>-9.0881344948484024</v>
       </c>
       <c r="E25">
         <f t="shared" ca="1" si="5"/>
-        <v>-21.995758080439344</v>
+        <v>-12.306840535323751</v>
       </c>
       <c r="G25">
         <f t="shared" ca="1" si="3"/>
-        <v>32.095088080979913</v>
+        <v>5.9322131787389196</v>
       </c>
       <c r="H25">
         <f t="shared" ca="1" si="4"/>
-        <v>124.59260041478856</v>
+        <v>22.135183172477451</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
@@ -3402,23 +3402,23 @@
       </c>
       <c r="C26">
         <f t="shared" ca="1" si="1"/>
-        <v>1.193065753965513</v>
+        <v>2.8823516890362058</v>
       </c>
       <c r="D26">
         <f t="shared" ca="1" si="2"/>
-        <v>0.69834744053311582</v>
+        <v>7.5563269610367367</v>
       </c>
       <c r="E26">
         <f t="shared" ref="E26:E35" ca="1" si="6">A26*C26+B26</f>
-        <v>-1.4208027381034611</v>
+        <v>3.6470550671086173</v>
       </c>
       <c r="G26">
         <f t="shared" ref="G26:G35" ca="1" si="7">C26*C26</f>
-        <v>1.423405893285298</v>
+        <v>8.3079512592898688</v>
       </c>
       <c r="H26">
         <f t="shared" ref="H26:H35" ca="1" si="8">C26*D26</f>
-        <v>0.83317441566952799</v>
+        <v>21.779991779054058</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.25">
@@ -3430,23 +3430,23 @@
       </c>
       <c r="C27">
         <f t="shared" ca="1" si="1"/>
-        <v>-8.7396015422229123</v>
+        <v>5.869794339984665</v>
       </c>
       <c r="D27">
         <f t="shared" ca="1" si="2"/>
-        <v>-31.963842249024765</v>
+        <v>5.3021711998670007</v>
       </c>
       <c r="E27">
         <f t="shared" ca="1" si="6"/>
-        <v>-31.218804626668735</v>
+        <v>12.609383019953995</v>
       </c>
       <c r="G27">
         <f t="shared" ca="1" si="7"/>
-        <v>76.380635116825104</v>
+        <v>34.454485593716008</v>
       </c>
       <c r="H27">
         <f t="shared" ca="1" si="8"/>
-        <v>279.3512450149467</v>
+        <v>31.12265449860902</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.25">
@@ -3458,23 +3458,23 @@
       </c>
       <c r="C28">
         <f t="shared" ca="1" si="1"/>
-        <v>-5.8504340646699493</v>
+        <v>8.558082680191049</v>
       </c>
       <c r="D28">
         <f t="shared" ca="1" si="2"/>
-        <v>-17.519261579906498</v>
+        <v>22.612292848383756</v>
       </c>
       <c r="E28">
         <f t="shared" ca="1" si="6"/>
-        <v>-22.55130219400985</v>
+        <v>20.674248040573147</v>
       </c>
       <c r="G28">
         <f t="shared" ca="1" si="7"/>
-        <v>34.227578745050543</v>
+        <v>73.240779160986008</v>
       </c>
       <c r="H28">
         <f t="shared" ca="1" si="8"/>
-        <v>102.49528473494846</v>
+        <v>193.51787178516093</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.25">
@@ -3486,23 +3486,23 @@
       </c>
       <c r="C29">
         <f t="shared" ca="1" si="1"/>
-        <v>4.5563085794710005</v>
+        <v>3.6536566110692466</v>
       </c>
       <c r="D29">
         <f t="shared" ca="1" si="2"/>
-        <v>9.8546287789354583</v>
+        <v>12.089442264706967</v>
       </c>
       <c r="E29">
         <f t="shared" ca="1" si="6"/>
-        <v>8.6689257384130016</v>
+        <v>5.9609698332077397</v>
       </c>
       <c r="G29">
         <f t="shared" ca="1" si="7"/>
-        <v>20.759947871361046</v>
+        <v>13.349206631610011</v>
       </c>
       <c r="H29">
         <f t="shared" ca="1" si="8"/>
-        <v>44.90072965296546</v>
+        <v>44.170670654586573</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.25">
@@ -3514,23 +3514,23 @@
       </c>
       <c r="C30">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.50986669413980401</v>
+        <v>0.45377896356381697</v>
       </c>
       <c r="D30">
         <f t="shared" ca="1" si="2"/>
-        <v>-10.856846541179682</v>
+        <v>-7.4443975621264489</v>
       </c>
       <c r="E30">
         <f t="shared" ca="1" si="6"/>
-        <v>-6.529600082419412</v>
+        <v>-3.6386631093085491</v>
       </c>
       <c r="G30">
         <f t="shared" ca="1" si="7"/>
-        <v>0.25996404579305243</v>
+        <v>0.20591534777305193</v>
       </c>
       <c r="H30">
         <f t="shared" ca="1" si="8"/>
-        <v>5.5355444547344499</v>
+        <v>-3.3781110100987459</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.25">
@@ -3542,23 +3542,23 @@
       </c>
       <c r="C31">
         <f t="shared" ca="1" si="1"/>
-        <v>-0.24261640966571107</v>
+        <v>9.7834398893335006</v>
       </c>
       <c r="D31">
         <f t="shared" ca="1" si="2"/>
-        <v>-8.338762010397561</v>
+        <v>26.715761935747508</v>
       </c>
       <c r="E31">
         <f t="shared" ca="1" si="6"/>
-        <v>-5.7278492289971332</v>
+        <v>24.350319668000502</v>
       </c>
       <c r="G31">
         <f t="shared" ca="1" si="7"/>
-        <v>5.8862722239080144E-2</v>
+        <v>95.715696068201893</v>
       </c>
       <c r="H31">
         <f t="shared" ca="1" si="8"/>
-        <v>2.0231205000194832</v>
+        <v>261.37205099612976</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
@@ -3570,23 +3570,23 @@
       </c>
       <c r="C32">
         <f t="shared" ca="1" si="1"/>
-        <v>7.9304074553934676</v>
+        <v>-1.4262116945963292</v>
       </c>
       <c r="D32">
         <f t="shared" ca="1" si="2"/>
-        <v>19.568059472444205</v>
+        <v>-10.116711522812965</v>
       </c>
       <c r="E32">
         <f t="shared" ca="1" si="6"/>
-        <v>18.791222366180403</v>
+        <v>-9.2786350837889877</v>
       </c>
       <c r="G32">
         <f t="shared" ca="1" si="7"/>
-        <v>62.89136240856029</v>
+        <v>2.0340797978033329</v>
       </c>
       <c r="H32">
         <f t="shared" ca="1" si="8"/>
-        <v>155.18268472785428</v>
+        <v>14.428572284693288</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.25">
@@ -3598,23 +3598,23 @@
       </c>
       <c r="C33">
         <f t="shared" ca="1" si="1"/>
-        <v>6.2014988414571981</v>
+        <v>-9.2896050878444196</v>
       </c>
       <c r="D33">
         <f t="shared" ca="1" si="2"/>
-        <v>5.8368880554364218</v>
+        <v>-37.228751217942261</v>
       </c>
       <c r="E33">
         <f t="shared" ca="1" si="6"/>
-        <v>13.604496524371594</v>
+        <v>-32.868815263533257</v>
       </c>
       <c r="G33">
         <f t="shared" ca="1" si="7"/>
-        <v>38.458587880594969</v>
+        <v>86.296762688104934</v>
       </c>
       <c r="H33">
         <f t="shared" ca="1" si="8"/>
-        <v>36.197454513504326</v>
+        <v>345.84039672829056</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.25">
@@ -3626,23 +3626,23 @@
       </c>
       <c r="C34">
         <f t="shared" ca="1" si="1"/>
-        <v>-3.5243415840914105</v>
+        <v>-9.5712704911017283</v>
       </c>
       <c r="D34">
         <f t="shared" ca="1" si="2"/>
-        <v>-19.453280391876987</v>
+        <v>-41.364246226299151</v>
       </c>
       <c r="E34">
         <f t="shared" ca="1" si="6"/>
-        <v>-15.573024752274232</v>
+        <v>-33.713811473305185</v>
       </c>
       <c r="G34">
         <f t="shared" ca="1" si="7"/>
-        <v>12.420983601355953</v>
+        <v>91.609218813834715</v>
       </c>
       <c r="H34">
         <f t="shared" ca="1" si="8"/>
-        <v>68.560005032082117</v>
+        <v>395.90838929244308</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.25">
@@ -3654,23 +3654,23 @@
       </c>
       <c r="C35">
         <f t="shared" ca="1" si="1"/>
-        <v>6.0344773562181402</v>
+        <v>-6.7105313167625198</v>
       </c>
       <c r="D35">
         <f t="shared" ca="1" si="2"/>
-        <v>19.152451294974313</v>
+        <v>-23.218327756788241</v>
       </c>
       <c r="E35">
         <f t="shared" ca="1" si="6"/>
-        <v>13.103432068654421</v>
+        <v>-25.131593950287559</v>
       </c>
       <c r="G35">
         <f t="shared" ca="1" si="7"/>
-        <v>36.414916962709476</v>
+        <v>45.031230553250516</v>
       </c>
       <c r="H35">
         <f t="shared" ca="1" si="8"/>
-        <v>115.57503365559329</v>
+        <v>155.80731553478395</v>
       </c>
     </row>
   </sheetData>

</xml_diff>